<commit_message>
app deletes temp files on exit
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -91,7 +91,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>24</row>
+      <row>25</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="11430000" cy="4762500"/>
@@ -116,7 +116,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>49</row>
+      <row>50</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="11430000" cy="4762500"/>
@@ -141,7 +141,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>74</row>
+      <row>75</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="11430000" cy="4762500"/>
@@ -166,7 +166,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>99</row>
+      <row>100</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="11430000" cy="4762500"/>
@@ -479,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A100"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,10 +488,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1"/>
-    <row r="25" spans="1:1"/>
-    <row r="50" spans="1:1"/>
-    <row r="75" spans="1:1"/>
-    <row r="100" spans="1:1"/>
+    <row r="26" spans="1:1"/>
+    <row r="51" spans="1:1"/>
+    <row r="76" spans="1:1"/>
+    <row r="101" spans="1:1"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
import/export config, completed adv settings
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Race Site SPectrum Test" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Race Site Spectrum Test" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
@@ -77,131 +77,6 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>25</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="11430000" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr descr="Picture" id="2" name="Image 2"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>50</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="11430000" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr descr="Picture" id="3" name="Image 3"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>75</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="11430000" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr descr="Picture" id="4" name="Image 4"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>100</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="11430000" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr descr="Picture" id="5" name="Image 5"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>125</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="11430000" cy="4762500"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr descr="Picture" id="6" name="Image 6"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -504,7 +379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A126"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,11 +388,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1"/>
-    <row r="26" spans="1:1"/>
-    <row r="51" spans="1:1"/>
-    <row r="76" spans="1:1"/>
-    <row r="101" spans="1:1"/>
-    <row r="126" spans="1:1"/>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <drawing r:id="rId1"/>

</xml_diff>